<commit_message>
Ajout gestion altitude Vérifier précision des valeurs (troncature?)
</commit_message>
<xml_diff>
--- a/étude faisabilité.xlsx
+++ b/étude faisabilité.xlsx
@@ -162,12 +162,6 @@
     <t>studioSPORT</t>
   </si>
   <si>
-    <t>http://www.studiosport.fr/antenne-pinwheel-p-998.html</t>
-  </si>
-  <si>
-    <t>Antenne PinWheel SL 5,8 Ghz - SMA</t>
-  </si>
-  <si>
     <t>antenne vidéo</t>
   </si>
   <si>
@@ -245,6 +239,12 @@
       </rPr>
       <t>voir plutôt pour du 4S</t>
     </r>
+  </si>
+  <si>
+    <t>http://www.hobbyking.com/hobbyking/store/__27750__5_8GHz_Circular_Polarized_Clover_Leaf_spiroNet_Antenna.html</t>
+  </si>
+  <si>
+    <t>ImmersionRC 5.8GHz Circular Polarized spiroNet Antenna</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -511,27 +511,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -549,7 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -866,7 +850,7 @@
   <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +865,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -915,7 +899,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8">
@@ -932,18 +916,18 @@
         <v>3.68</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -951,7 +935,7 @@
       <c r="C5" s="8">
         <v>38.5</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>2</v>
       </c>
       <c r="E5" s="8">
@@ -960,101 +944,101 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="20">
+      <c r="B6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="19">
         <v>7.71</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <f t="shared" ref="E6:E11" si="0">C6*D6</f>
         <v>7.71</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="19">
         <v>1.51</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="19">
         <v>6.95</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="19">
         <v>1.55</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:9" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19">
         <v>8.1</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>1</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="19">
         <f>C8*D8</f>
         <v>8.1</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <v>0.88</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>59</v>
+      <c r="I8" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1062,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
@@ -1078,11 +1062,11 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1147,10 +1131,10 @@
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="6">
         <v>39.99</v>
@@ -1166,13 +1150,13 @@
         <v>6.5</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1238,7 +1222,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -1254,13 +1238,13 @@
         <v>40</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>44</v>
+      <c r="I20" s="12" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1270,23 +1254,23 @@
       <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1300,12 +1284,12 @@
     <hyperlink ref="I7" r:id="rId4"/>
     <hyperlink ref="I8" r:id="rId5" display="http://www.ebay.fr/itm/BMP085-Temperature-Altimeter-Atmospheric-Pressure-Sensor-Board-for-Arduino-DIY-/231013228106?pt=UK_BOI_Electrical_Components_Supplies_ET&amp;hash=item35c9761e4a"/>
     <hyperlink ref="I19" r:id="rId6"/>
-    <hyperlink ref="I20" r:id="rId7"/>
-    <hyperlink ref="I12" r:id="rId8"/>
-    <hyperlink ref="I4" r:id="rId9"/>
-    <hyperlink ref="I5" r:id="rId10"/>
-    <hyperlink ref="I9" r:id="rId11"/>
-    <hyperlink ref="C26" r:id="rId12"/>
+    <hyperlink ref="I12" r:id="rId7"/>
+    <hyperlink ref="I4" r:id="rId8"/>
+    <hyperlink ref="I5" r:id="rId9"/>
+    <hyperlink ref="I9" r:id="rId10"/>
+    <hyperlink ref="C26" r:id="rId11"/>
+    <hyperlink ref="I20" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>

</xml_diff>